<commit_message>
57 - ERD maken" (1123) ----$ Niek Vandael "<No comment>" 12-Apr-2016 09:43 PM Changes: ---c- /italent/documents/analyse/ClassDiagram/KlassenDiagram.vsdx Work items: (1124) 50 "Klassediagrammen maken ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=57 )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/use-cases/use_cases.xlsx
+++ b/italent/documents/analyse/use-cases/use_cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="10665" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="10665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Algemeen" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="92">
   <si>
     <t>Naam</t>
   </si>
@@ -104,15 +104,6 @@
     <t>liken van de projecten in de projectenlijst</t>
   </si>
   <si>
-    <t>1. Gebruiker klikt op 'like' bij een bepaald project
-2. Systeem kijkt na of de gebruiker het project reeds geliked heeft
-3. Systeem toont de geupdate pagina met nieuwe aantal likes en melding dat de gebruiker dit project heeft geliked</t>
-  </si>
-  <si>
-    <t>[Gebruiker heeft reeds geliked]
-1. Systeem laat de melding zien "reeds geliked"</t>
-  </si>
-  <si>
     <t>Inschrijven op een bepaald project</t>
   </si>
   <si>
@@ -132,10 +123,6 @@
   </si>
   <si>
     <t>use case 'projectenlijst tonen' of 'projectdetails bekijken' werd successvol afgerond.</t>
-  </si>
-  <si>
-    <t>1. Gebruiker klikt op 'meer info' bij een bepaald project
-2. Systeem laad de detailpagina en laatgegevens van het gekozen project zien</t>
   </si>
   <si>
     <t>1. Gebruiker klikt 'inschrijven' bij een bepaald project
@@ -272,10 +259,6 @@
 7. Systeem toont melding 'successvol opgeslaan'</t>
   </si>
   <si>
-    <t>[Gegevens niet goed gevalideert]
-1. Systeem laat melding zien waarom de validatie mislukt</t>
-  </si>
-  <si>
     <t>Projecten beheren</t>
   </si>
   <si>
@@ -306,10 +289,6 @@
     <t>Er werd een project verwijderd</t>
   </si>
   <si>
-    <t>[Project is reeds gevalideert]
-1. Systeem toont melding: 'gevalideerde projecten kunnen niet meer verwijderd worden'</t>
-  </si>
-  <si>
     <t>Projecten volgen</t>
   </si>
   <si>
@@ -359,6 +338,36 @@
   <si>
     <t>1. Gebruiker kiest voor 'lopende projecten bekijken'
 2. Systeem toont projectenlijst van lopende projecten</t>
+  </si>
+  <si>
+    <t>Bestaande PXL student/docent of gast</t>
+  </si>
+  <si>
+    <t>1. Gebruiker klikt op 'like' bij een bepaald project
+2. Systeem kijkt na of de gebruiker het project reeds geliket heeft
+3. Systeem toont de geupdate pagina met nieuwe aantal likes en melding dat de gebruiker dit project heeft geliket</t>
+  </si>
+  <si>
+    <t>[Gebruiker heeft reeds geliket]
+1. Systeem gaat de like verwijderen</t>
+  </si>
+  <si>
+    <t>Use case 'projectenlijst tonen' werd successvol afgerond.</t>
+  </si>
+  <si>
+    <t>1. Gebruiker klikt op 'meer info' bij een bepaald project
+2. Systeem laad de detailpagina en laat gegevens van het gekozen project zien</t>
+  </si>
+  <si>
+    <t>use case 'projectdetails bekijken' werd successvol afgerond en het project is volledig geverifieerd</t>
+  </si>
+  <si>
+    <t>[Gegevens niet goed gevalideerd]
+1. Systeem laat melding zien waarom de validatie mislukt</t>
+  </si>
+  <si>
+    <t>[Project is reeds gevalideerd]
+1. Systeem toont melding: 'gevalideerde projecten kunnen niet meer verwijderd worden'</t>
   </si>
 </sst>
 </file>
@@ -474,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -505,6 +514,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -817,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:B80"/>
+    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +887,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +895,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -923,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +946,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -966,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1073,7 +1088,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1081,7 +1096,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1089,7 +1104,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1100,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1147,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1140,7 +1155,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1148,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1165,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1181,7 +1196,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,12 +1207,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1205,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1228,7 @@
         <v>6</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1221,7 +1236,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1230,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1246,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1270,7 +1285,7 @@
         <v>5</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1295,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1311,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1327,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1335,7 +1350,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,7 +1358,7 @@
         <v>6</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1360,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1400,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1423,7 @@
         <v>6</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1426,77 +1441,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C108"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92:C99"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="69" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="str">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="str">
         <f>Algemeen!A1</f>
         <v>Naam</v>
       </c>
-      <c r="C2" s="3" t="str">
+      <c r="B2" s="3" t="str">
         <f>Algemeen!B1</f>
         <v>Aanmelden</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="str">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>Algemeen!A2</f>
         <v>ID</v>
       </c>
-      <c r="C3" s="5">
+      <c r="B3" s="5">
         <f>Algemeen!B2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="str">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="str">
         <f>Algemeen!A3</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C4" s="7" t="str">
+      <c r="B4" s="7" t="str">
         <f>Algemeen!B3</f>
         <v>Aanmelden op iTalent</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="str">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>Algemeen!A4</f>
         <v>Actoren</v>
       </c>
-      <c r="C5" s="5" t="str">
+      <c r="B5" s="5" t="str">
         <f>Algemeen!B4</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="str">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="str">
         <f>Algemeen!A5</f>
         <v>Preconditie</v>
       </c>
-      <c r="C6" s="9" t="str">
+      <c r="B6" s="9" t="str">
         <f>Algemeen!B5</f>
         <v xml:space="preserve">Loginscherm is zichtbaar
 Gebruiker kent zijn gebruikersnaam en wachtwoord
 </v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="str">
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>Algemeen!A6</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C7" s="10" t="str">
+      <c r="B7" s="10" t="str">
         <f>Algemeen!B6</f>
         <v>1. Gebruiker voert gebruikersnaam en wachtwoord in.
 2. Systeem controleert de gegevens
@@ -1504,22 +1520,22 @@
 3. Systeem toont projecten en de aangemeldde gebruikersgegevens</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="str">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="str">
         <f>Algemeen!A7</f>
         <v>Postconditie</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="B8" s="7" t="str">
         <f>Algemeen!B7</f>
         <v>Gebruiker is aangemeld en ziet zijn gegevens + er werd een sessie gemaakt voor de gebruiker</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="str">
+    <row r="9" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="str">
         <f>Algemeen!A8</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C9" s="11" t="str">
+      <c r="B9" s="11" t="str">
         <f>Algemeen!B8</f>
         <v>[Logingegevens verkeerd]
 1. iTalent geeft aan dat gegevens incorrect zijn
@@ -1527,405 +1543,386 @@
 3. ga verder met stap 2 van het hoofdscenario</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="str">
-        <f>Algemeen!A10</f>
-        <v>Naam</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f>Algemeen!B10</f>
-        <v>Projectenlijst tonen</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="str">
-        <f>Algemeen!A11</f>
-        <v>ID</v>
-      </c>
-      <c r="C12" s="5">
-        <f>Algemeen!B11</f>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="str">
-        <f>Algemeen!A12</f>
-        <v>Samenvatting</v>
-      </c>
-      <c r="C13" s="7" t="str">
-        <f>Algemeen!B12</f>
-        <v>Tonen van projectenlijst</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="str">
-        <f>Algemeen!A13</f>
-        <v>Actoren</v>
-      </c>
-      <c r="C14" s="5" t="str">
-        <f>Algemeen!B13</f>
-        <v>Bestaande PXL student/docent</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="str">
-        <f>Algemeen!A14</f>
-        <v>Preconditie</v>
-      </c>
-      <c r="C15" s="9" t="str">
-        <f>Algemeen!B14</f>
-        <v>use case 'aanmelden' werd successvol afgerond of er is een actieve sessie voor de gebruiker</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="str">
-        <f>Algemeen!A15</f>
-        <v>Hoofdscenario</v>
-      </c>
-      <c r="C16" s="10" t="str">
-        <f>Algemeen!B15</f>
-        <v>1. Systeem toont projectenlijst</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="str">
-        <f>Algemeen!A16</f>
-        <v>Postconditie</v>
-      </c>
-      <c r="C17" s="7" t="str">
-        <f>Algemeen!B16</f>
-        <v>Gebruiker ziet een lijst van de projecten</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="str">
-        <f>Algemeen!A17</f>
-        <v>Alternatief scenario</v>
-      </c>
-      <c r="C18" s="11" t="str">
-        <f>Algemeen!B17</f>
-        <v>[Geen projecten beschikbaar]
-1. Systeem laat de melding zien "geen projecten beschikbaar"</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="str">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="str">
         <f>Algemeen!A19</f>
         <v>Naam</v>
       </c>
-      <c r="C20" s="3" t="str">
+      <c r="B20" s="3" t="str">
         <f>Algemeen!B19</f>
         <v>Projectenlijst sorteren</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="str">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="str">
         <f>Algemeen!A20</f>
         <v>ID</v>
       </c>
-      <c r="C21" s="5">
+      <c r="B21" s="5">
         <f>Algemeen!B20</f>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="str">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="str">
         <f>Algemeen!A21</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C22" s="7" t="str">
+      <c r="B22" s="7" t="str">
         <f>Algemeen!B21</f>
         <v>Sorteren van de projecten in de projectenlijst</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="str">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="str">
         <f>Algemeen!A22</f>
         <v>Actoren</v>
       </c>
-      <c r="C23" s="5" t="str">
+      <c r="B23" s="5" t="str">
         <f>Algemeen!B22</f>
-        <v>Bestaande PXL student/docent</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="str">
+        <v>Bestaande PXL student/docent of gast</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="str">
         <f>Algemeen!A23</f>
         <v>Preconditie</v>
       </c>
-      <c r="C24" s="9" t="str">
+      <c r="B24" s="9" t="str">
         <f>Algemeen!B23</f>
         <v>use case 'projectenlijst tonen' werd successvol afgerond.</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="str">
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="str">
         <f>Algemeen!A24</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C25" s="10" t="str">
+      <c r="B25" s="10" t="str">
         <f>Algemeen!B24</f>
         <v>1. Gebruiker kiest een sorteerweergave
 2. Systeem sorteert de projecten aan de hand van de gekozen sortering
 3. Gebruiker ziet een gesorteerde lijst</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="str">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="str">
         <f>Algemeen!A25</f>
         <v>Postconditie</v>
       </c>
-      <c r="C26" s="7" t="str">
+      <c r="B26" s="7" t="str">
         <f>Algemeen!B25</f>
         <v>Gebruiker ziet een lijst van de projecten</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="str">
+    <row r="27" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="str">
         <f>Algemeen!A26</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C27" s="11" t="str">
+      <c r="B27" s="11" t="str">
         <f>Algemeen!B26</f>
         <v>[Geen projecten beschikbaar]
 1. Systeem laat de melding zien "geen projecten beschikbaar"</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2" t="str">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="str">
         <f>Algemeen!A28</f>
         <v>Naam</v>
       </c>
-      <c r="C29" s="3" t="str">
+      <c r="B29" s="3" t="str">
         <f>Algemeen!B28</f>
         <v>Projecten liken</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="str">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="str">
         <f>Algemeen!A29</f>
         <v>ID</v>
       </c>
-      <c r="C30" s="5">
+      <c r="B30" s="5">
         <f>Algemeen!B29</f>
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="str">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="str">
         <f>Algemeen!A30</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C31" s="7" t="str">
+      <c r="B31" s="7" t="str">
         <f>Algemeen!B30</f>
         <v>liken van de projecten in de projectenlijst</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="str">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="str">
         <f>Algemeen!A31</f>
         <v>Actoren</v>
       </c>
-      <c r="C32" s="5" t="str">
+      <c r="B32" s="5" t="str">
         <f>Algemeen!B31</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="str">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="str">
         <f>Algemeen!A32</f>
         <v>Preconditie</v>
       </c>
-      <c r="C33" s="9" t="str">
+      <c r="B33" s="9" t="str">
         <f>Algemeen!B32</f>
         <v>use case 'projectenlijst tonen' werd successvol afgerond.</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="str">
+    <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="str">
         <f>Algemeen!A33</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C34" s="10" t="str">
+      <c r="B34" s="10" t="str">
         <f>Algemeen!B33</f>
         <v>1. Gebruiker klikt op 'like' bij een bepaald project
-2. Systeem kijkt na of de gebruiker het project reeds geliked heeft
-3. Systeem toont de geupdate pagina met nieuwe aantal likes en melding dat de gebruiker dit project heeft geliked</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="str">
+2. Systeem kijkt na of de gebruiker het project reeds geliket heeft
+3. Systeem toont de geupdate pagina met nieuwe aantal likes en melding dat de gebruiker dit project heeft geliket</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="str">
         <f>Algemeen!A34</f>
         <v>Postconditie</v>
       </c>
-      <c r="C35" s="7" t="str">
+      <c r="B35" s="7" t="str">
         <f>Algemeen!B34</f>
         <v>Likes van een project zijn geupdatet</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="8" t="str">
+    <row r="36" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="str">
         <f>Algemeen!A35</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C36" s="11" t="str">
+      <c r="B36" s="11" t="str">
         <f>Algemeen!B35</f>
-        <v>[Gebruiker heeft reeds geliked]
-1. Systeem laat de melding zien "reeds geliked"</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="str">
+        <v>[Gebruiker heeft reeds geliket]
+1. Systeem gaat de like verwijderen</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="str">
         <f>Algemeen!A37</f>
         <v>Naam</v>
       </c>
-      <c r="C38" s="3" t="str">
+      <c r="B38" s="3" t="str">
         <f>Algemeen!B37</f>
         <v>Projectdetails bekijken</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="str">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="str">
         <f>Algemeen!A38</f>
         <v>ID</v>
       </c>
-      <c r="C39" s="5">
+      <c r="B39" s="5">
         <f>Algemeen!B38</f>
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="str">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="str">
         <f>Algemeen!A39</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C40" s="7" t="str">
+      <c r="B40" s="7" t="str">
         <f>Algemeen!B39</f>
         <v>Details van een project bekijken</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="str">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="str">
         <f>Algemeen!A40</f>
         <v>Actoren</v>
       </c>
-      <c r="C41" s="5" t="str">
+      <c r="B41" s="5" t="str">
         <f>Algemeen!B40</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="str">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="str">
         <f>Algemeen!A41</f>
         <v>Preconditie</v>
       </c>
-      <c r="C42" s="9" t="str">
+      <c r="B42" s="9" t="str">
         <f>Algemeen!B41</f>
-        <v>use case 'projectenlijst tonen' werd successvol afgerond.</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="str">
+        <v>Use case 'projectenlijst tonen' werd successvol afgerond.</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="str">
         <f>Algemeen!A42</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C43" s="10" t="str">
+      <c r="B43" s="10" t="str">
         <f>Algemeen!B42</f>
         <v>1. Gebruiker klikt op 'meer info' bij een bepaald project
-2. Systeem laad de detailpagina en laatgegevens van het gekozen project zien</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="str">
+2. Systeem laad de detailpagina en laat gegevens van het gekozen project zien</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="str">
         <f>Algemeen!A43</f>
         <v>Postconditie</v>
       </c>
-      <c r="C44" s="7" t="str">
+      <c r="B44" s="7" t="str">
         <f>Algemeen!B43</f>
         <v>Gebruiker ziet de detail van een project</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="8" t="str">
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="str">
         <f>Algemeen!A44</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C45" s="11">
-        <f>Algemeen!B44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="2" t="str">
+      <c r="B45" s="11"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="str">
         <f>Algemeen!A46</f>
         <v>Naam</v>
       </c>
-      <c r="C47" s="3" t="str">
+      <c r="B47" s="3" t="str">
         <f>Algemeen!B46</f>
         <v>Inschrijven op een project</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="str">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="str">
         <f>Algemeen!A47</f>
         <v>ID</v>
       </c>
-      <c r="C48" s="5">
+      <c r="B48" s="5">
         <f>Algemeen!B47</f>
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="str">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="str">
         <f>Algemeen!A48</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C49" s="7" t="str">
+      <c r="B49" s="7" t="str">
         <f>Algemeen!B48</f>
         <v>Inschrijven op een bepaald project</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="str">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="str">
         <f>Algemeen!A49</f>
         <v>Actoren</v>
       </c>
-      <c r="C50" s="5" t="str">
+      <c r="B50" s="5" t="str">
         <f>Algemeen!B49</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="str">
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="str">
         <f>Algemeen!A50</f>
         <v>Preconditie</v>
       </c>
-      <c r="C51" s="9" t="str">
+      <c r="B51" s="9" t="str">
         <f>Algemeen!B50</f>
-        <v>use case 'projectenlijst tonen' of 'projectdetails bekijken' werd successvol afgerond.</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="str">
+        <v>use case 'projectdetails bekijken' werd successvol afgerond en het project is volledig geverifieerd</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="str">
         <f>Algemeen!A51</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C52" s="10" t="str">
+      <c r="B52" s="10" t="str">
         <f>Algemeen!B51</f>
         <v>1. Gebruiker klikt 'inschrijven' bij een bepaald project
 2. Systeem controleert of de gebruiker kan inschrijven voor dit project
@@ -1934,22 +1931,22 @@
 5. Systeem toont melding aan de gebruiker: 'succesvol toegevoegd'</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="6" t="str">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="str">
         <f>Algemeen!A52</f>
         <v>Postconditie</v>
       </c>
-      <c r="C53" s="7" t="str">
+      <c r="B53" s="7" t="str">
         <f>Algemeen!B52</f>
         <v>Gebruiker is inschreven op een project</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="8" t="str">
+    <row r="54" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="str">
         <f>Algemeen!A53</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C54" s="11" t="str">
+      <c r="B54" s="11" t="str">
         <f>Algemeen!B53</f>
         <v>[Gebruiker is reeds ingeschreven op een ander project]
 1. Systeem laat melding zien: 'u bent reeds ingescrheven op een ander project'
@@ -1957,447 +1954,447 @@
 2. Systeem laat melding zien: 'u kan niet inschrijven voor dit project'</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55">
+    <row r="55" spans="1:2" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55">
         <f>Algemeen!B54</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="B56" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="63" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="5">
+      <c r="B66" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="2" t="str">
+      <c r="B72" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="str">
         <f>Algemeen!A55</f>
         <v>Naam</v>
       </c>
-      <c r="C74" s="3" t="str">
+      <c r="B74" s="3" t="str">
         <f>Algemeen!B55</f>
         <v>Afgeronde projecten tonen</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="str">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="str">
         <f>Algemeen!A56</f>
         <v>ID</v>
       </c>
-      <c r="C75" s="5">
+      <c r="B75" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="6" t="str">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="str">
         <f>Algemeen!A57</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C76" s="7" t="str">
+      <c r="B76" s="7" t="str">
         <f>Algemeen!B57</f>
         <v>Tonen van afgeronde projectenlijst</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="str">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="str">
         <f>Algemeen!A58</f>
         <v>Actoren</v>
       </c>
-      <c r="C77" s="5" t="str">
+      <c r="B77" s="5" t="str">
         <f>Algemeen!B58</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="6" t="str">
+    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="str">
         <f>Algemeen!A59</f>
         <v>Preconditie</v>
       </c>
-      <c r="C78" s="9" t="str">
+      <c r="B78" s="9" t="str">
         <f>Algemeen!B59</f>
         <v>use case 'aanmelden' werd successvol afgerond of er is een actieve sessie voor de gebruiker</v>
       </c>
     </row>
-    <row r="79" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="str">
+    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="str">
         <f>Algemeen!A60</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C79" s="10" t="str">
+      <c r="B79" s="10" t="str">
         <f>Algemeen!B60</f>
         <v>1. Gebruiker kiest voor 'afgeronde projecten bekijken'
 2. Systeem toont projectenlijst van afgeronde projecten</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="6" t="str">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="str">
         <f>Algemeen!A61</f>
         <v>Postconditie</v>
       </c>
-      <c r="C80" s="7" t="str">
+      <c r="B80" s="7" t="str">
         <f>Algemeen!B61</f>
         <v>Gebruiker ziet een lijst van de afgeronde projecten</v>
       </c>
     </row>
-    <row r="81" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="8" t="str">
+    <row r="81" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="8" t="str">
         <f>Algemeen!A62</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C81" s="11" t="str">
+      <c r="B81" s="11" t="str">
         <f>Algemeen!B62</f>
         <v>[Geen projecten beschikbaar]
 1. Systeem laat de melding zien "geen projecten beschikbaar"</v>
       </c>
     </row>
-    <row r="82" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="2" t="s">
+    <row r="82" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+      <c r="B83" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C84" s="5">
+      <c r="B84" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="6" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C85" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+      <c r="B85" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="6" t="s">
+      <c r="B86" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+      <c r="B87" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C88" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="6" t="s">
+      <c r="B88" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="8" t="s">
+      <c r="B89" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C90" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="2" t="str">
+      <c r="B90" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="str">
         <f>Algemeen!A64</f>
         <v>Naam</v>
       </c>
-      <c r="C92" s="3" t="str">
+      <c r="B92" s="3" t="str">
         <f>Algemeen!B64</f>
         <v>Projecten volgen</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="str">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="str">
         <f>Algemeen!A65</f>
         <v>ID</v>
       </c>
-      <c r="C93" s="5">
+      <c r="B93" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="6" t="str">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="str">
         <f>Algemeen!A66</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C94" s="7" t="str">
+      <c r="B94" s="7" t="str">
         <f>Algemeen!B66</f>
         <v>Tonen van projecten waarop de gebruiker gesubscribed is</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="str">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="str">
         <f>Algemeen!A67</f>
         <v>Actoren</v>
       </c>
-      <c r="C95" s="5" t="str">
+      <c r="B95" s="5" t="str">
         <f>Algemeen!B67</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="6" t="str">
+    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="str">
         <f>Algemeen!A68</f>
         <v>Preconditie</v>
       </c>
-      <c r="C96" s="9" t="str">
+      <c r="B96" s="9" t="str">
         <f>Algemeen!B68</f>
         <v>use case 'aanmelden' werd successvol afgerond of er is een actieve sessie voor de gebruiker</v>
       </c>
     </row>
-    <row r="97" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="str">
+    <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="str">
         <f>Algemeen!A69</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C97" s="10" t="str">
+      <c r="B97" s="10" t="str">
         <f>Algemeen!B69</f>
         <v>1. Gebruiker kiest voor 'huidige projecten bekijken'
 2. Systeem toont projectenlijst waarop de gebruiker gesubscribed is</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="6" t="str">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="str">
         <f>Algemeen!A70</f>
         <v>Postconditie</v>
       </c>
-      <c r="C98" s="7" t="str">
+      <c r="B98" s="7" t="str">
         <f>Algemeen!B70</f>
         <v>Gebruiker ziet een lijst van de afgeronde projecten</v>
       </c>
     </row>
-    <row r="99" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="8" t="str">
+    <row r="99" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="str">
         <f>Algemeen!A71</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C99" s="11" t="str">
+      <c r="B99" s="11" t="str">
         <f>Algemeen!B71</f>
         <v>[Geen projecten beschikbaar]
 1. Systeem laat de melding zien "geen projecten beschikbaar"</v>
       </c>
     </row>
-    <row r="100" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="2" t="str">
+    <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="str">
         <f>Algemeen!A73</f>
         <v>Naam</v>
       </c>
-      <c r="C101" s="3" t="str">
+      <c r="B101" s="3" t="str">
         <f>Algemeen!B73</f>
         <v>Lopende projecten tonen</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="str">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="str">
         <f>Algemeen!A74</f>
         <v>ID</v>
       </c>
-      <c r="C102" s="5">
+      <c r="B102" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="6" t="str">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="str">
         <f>Algemeen!A75</f>
         <v>Samenvatting</v>
       </c>
-      <c r="C103" s="7" t="str">
+      <c r="B103" s="7" t="str">
         <f>Algemeen!B75</f>
         <v>Tonen van lopende projectenlijst</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="str">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="str">
         <f>Algemeen!A76</f>
         <v>Actoren</v>
       </c>
-      <c r="C104" s="5" t="str">
+      <c r="B104" s="5" t="str">
         <f>Algemeen!B76</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="6" t="str">
+    <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="str">
         <f>Algemeen!A77</f>
         <v>Preconditie</v>
       </c>
-      <c r="C105" s="9" t="str">
+      <c r="B105" s="9" t="str">
         <f>Algemeen!B77</f>
         <v>use case 'aanmelden' werd successvol afgerond of er is een actieve sessie voor de gebruiker</v>
       </c>
     </row>
-    <row r="106" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="str">
+    <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="str">
         <f>Algemeen!A78</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="C106" s="10" t="str">
+      <c r="B106" s="10" t="str">
         <f>Algemeen!B78</f>
         <v>1. Gebruiker kiest voor 'lopende projecten bekijken'
 2. Systeem toont projectenlijst van lopende projecten</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="6" t="str">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="str">
         <f>Algemeen!A79</f>
         <v>Postconditie</v>
       </c>
-      <c r="C107" s="7" t="str">
+      <c r="B107" s="7" t="str">
         <f>Algemeen!B79</f>
         <v>Gebruiker ziet een lijst van de lopende projecten</v>
       </c>
     </row>
-    <row r="108" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="8" t="str">
+    <row r="108" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="8" t="str">
         <f>Algemeen!A80</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="C108" s="11" t="str">
+      <c r="B108" s="11" t="str">
         <f>Algemeen!B80</f>
         <v>[Geen projecten beschikbaar]
 1. Systeem laat de melding zien "geen projecten beschikbaar"</v>
@@ -2405,7 +2402,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2413,14 +2410,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:B98"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2551,7 +2548,7 @@
       </c>
       <c r="B13" s="5" t="str">
         <f>Algemeen!B13</f>
-        <v>Bestaande PXL student/docent</v>
+        <v>Bestaande PXL student/docent of gast</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2635,7 +2632,7 @@
       </c>
       <c r="B22" s="5" t="str">
         <f>Algemeen!B22</f>
-        <v>Bestaande PXL student/docent</v>
+        <v>Bestaande PXL student/docent of gast</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2742,8 +2739,8 @@
       <c r="B33" s="10" t="str">
         <f>Algemeen!B33</f>
         <v>1. Gebruiker klikt op 'like' bij een bepaald project
-2. Systeem kijkt na of de gebruiker het project reeds geliked heeft
-3. Systeem toont de geupdate pagina met nieuwe aantal likes en melding dat de gebruiker dit project heeft geliked</v>
+2. Systeem kijkt na of de gebruiker het project reeds geliket heeft
+3. Systeem toont de geupdate pagina met nieuwe aantal likes en melding dat de gebruiker dit project heeft geliket</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,8 +2760,8 @@
       </c>
       <c r="B35" s="11" t="str">
         <f>Algemeen!B35</f>
-        <v>[Gebruiker heeft reeds geliked]
-1. Systeem laat de melding zien "reeds geliked"</v>
+        <v>[Gebruiker heeft reeds geliket]
+1. Systeem gaat de like verwijderen</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2817,7 +2814,7 @@
       </c>
       <c r="B41" s="9" t="str">
         <f>Algemeen!B41</f>
-        <v>use case 'projectenlijst tonen' werd successvol afgerond.</v>
+        <v>Use case 'projectenlijst tonen' werd successvol afgerond.</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2828,7 +2825,7 @@
       <c r="B42" s="10" t="str">
         <f>Algemeen!B42</f>
         <v>1. Gebruiker klikt op 'meer info' bij een bepaald project
-2. Systeem laad de detailpagina en laatgegevens van het gekozen project zien</v>
+2. Systeem laad de detailpagina en laat gegevens van het gekozen project zien</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2901,7 +2898,7 @@
       </c>
       <c r="B50" s="9" t="str">
         <f>Algemeen!B50</f>
-        <v>use case 'projectenlijst tonen' of 'projectdetails bekijken' werd successvol afgerond.</v>
+        <v>use case 'projectdetails bekijken' werd successvol afgerond en het project is volledig geverifieerd</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3113,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -3129,7 +3126,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3137,7 +3134,7 @@
         <v>3</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3145,7 +3142,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -3153,7 +3150,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -3178,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -3194,7 +3191,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3202,7 +3199,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -3210,7 +3207,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -3218,7 +3215,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -3322,82 +3319,83 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D45"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="188" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="2" t="str">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="str">
         <f>Algemeen!A1</f>
         <v>Naam</v>
       </c>
-      <c r="D2" s="3" t="str">
+      <c r="B2" s="3" t="str">
         <f>Algemeen!B1</f>
         <v>Aanmelden</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="str">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>Algemeen!A2</f>
         <v>ID</v>
       </c>
-      <c r="D3" s="5">
+      <c r="B3" s="5">
         <f>Algemeen!B2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="str">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="str">
         <f>Algemeen!A3</f>
         <v>Samenvatting</v>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="B4" s="7" t="str">
         <f>Algemeen!B3</f>
         <v>Aanmelden op iTalent</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="str">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>Algemeen!A4</f>
         <v>Actoren</v>
       </c>
-      <c r="D5" s="5" t="str">
+      <c r="B5" s="5" t="str">
         <f>Algemeen!B4</f>
         <v>Bestaande PXL student/docent</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C6" s="6" t="str">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="str">
         <f>Algemeen!A5</f>
         <v>Preconditie</v>
       </c>
-      <c r="D6" s="9" t="str">
+      <c r="B6" s="9" t="str">
         <f>Algemeen!B5</f>
         <v xml:space="preserve">Loginscherm is zichtbaar
 Gebruiker kent zijn gebruikersnaam en wachtwoord
 </v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="str">
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>Algemeen!A6</f>
         <v>Hoofdscenario</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="B7" s="10" t="str">
         <f>Algemeen!B6</f>
         <v>1. Gebruiker voert gebruikersnaam en wachtwoord in.
 2. Systeem controleert de gegevens
@@ -3405,22 +3403,22 @@
 3. Systeem toont projecten en de aangemeldde gebruikersgegevens</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="6" t="str">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="str">
         <f>Algemeen!A7</f>
         <v>Postconditie</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="B8" s="7" t="str">
         <f>Algemeen!B7</f>
         <v>Gebruiker is aangemeld en ziet zijn gegevens + er werd een sessie gemaakt voor de gebruiker</v>
       </c>
     </row>
-    <row r="9" spans="3:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="8" t="str">
+    <row r="9" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="str">
         <f>Algemeen!A8</f>
         <v>Alternatief scenario</v>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="B9" s="11" t="str">
         <f>Algemeen!B8</f>
         <v>[Logingegevens verkeerd]
 1. iTalent geeft aan dat gegevens incorrect zijn
@@ -3428,268 +3426,269 @@
 3. ga verder met stap 2 van het hoofdscenario</v>
       </c>
     </row>
-    <row r="10" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="5">
+      <c r="B39" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B40" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="B42" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
+      <c r="B43" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="8" t="s">
+      <c r="B44" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="B45" s="11" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="3:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C43" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3697,14 +3696,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3743,7 +3742,7 @@
       </c>
       <c r="B4" s="5" t="str">
         <f>Algemeen!B13</f>
-        <v>Bestaande PXL student/docent</v>
+        <v>Bestaande PXL student/docent of gast</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3772,7 +3771,7 @@
         <v>Postconditie</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3823,7 +3822,7 @@
       </c>
       <c r="B14" s="5" t="str">
         <f>Algemeen!B22</f>
-        <v>Bestaande PXL student/docent</v>
+        <v>Bestaande PXL student/docent of gast</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3871,84 +3870,36 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="str">
-        <f>Algemeen!A37</f>
-        <v>Naam</v>
-      </c>
-      <c r="B20" s="3" t="str">
-        <f>Algemeen!B37</f>
-        <v>Projectdetails bekijken</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="str">
-        <f>Algemeen!A38</f>
-        <v>ID</v>
-      </c>
-      <c r="B21" s="5">
-        <v>3</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="str">
-        <f>Algemeen!A39</f>
-        <v>Samenvatting</v>
-      </c>
-      <c r="B22" s="7" t="str">
-        <f>Algemeen!B39</f>
-        <v>Details van een project bekijken</v>
-      </c>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="str">
-        <f>Algemeen!A40</f>
-        <v>Actoren</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <f>Algemeen!B40</f>
-        <v>Bestaande PXL student/docent</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="str">
-        <f>Algemeen!A41</f>
-        <v>Preconditie</v>
-      </c>
-      <c r="B24" s="9" t="str">
-        <f>Algemeen!B41</f>
-        <v>use case 'projectenlijst tonen' werd successvol afgerond.</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="str">
-        <f>Algemeen!A42</f>
-        <v>Hoofdscenario</v>
-      </c>
-      <c r="B25" s="10" t="str">
-        <f>Algemeen!B42</f>
-        <v>1. Gebruiker klikt op 'meer info' bij een bepaald project
-2. Systeem laad de detailpagina en laatgegevens van het gekozen project zien</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="10"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="str">
-        <f>Algemeen!A43</f>
-        <v>Postconditie</v>
-      </c>
-      <c r="B26" s="7" t="str">
-        <f>Algemeen!B43</f>
-        <v>Gebruiker ziet de detail van een project</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="str">
-        <f>Algemeen!A44</f>
-        <v>Alternatief scenario</v>
-      </c>
-      <c r="B27" s="11">
-        <f>Algemeen!B44</f>
-        <v>0</v>
-      </c>
+      <c r="A27" s="8"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4116,5 +4067,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>